<commit_message>
Changes to create maps
</commit_message>
<xml_diff>
--- a/src/PalazzuPlot.xlsx
+++ b/src/PalazzuPlot.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="184">
   <si>
     <t xml:space="preserve">Localidad</t>
   </si>
@@ -441,9 +441,6 @@
     <t xml:space="preserve">T2-BOTTOM2</t>
   </si>
   <si>
-    <t xml:space="preserve">T2-BOTTOM2B</t>
-  </si>
-  <si>
     <t xml:space="preserve">T2-BOTTOM3</t>
   </si>
   <si>
@@ -481,9 +478,6 @@
   </si>
   <si>
     <t xml:space="preserve">T2-BOTTOM15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T2-BOTTOM16</t>
   </si>
   <si>
     <t xml:space="preserve">T2-BOTTOM17</t>
@@ -1023,13 +1017,13 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F70" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U88" activeCellId="0" sqref="U88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5617,8 +5611,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5632,15 +5626,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S1048576"/>
+  <dimension ref="A1:S144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B181" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A181" activeCellId="0" sqref="A181"/>
-      <selection pane="topRight" activeCell="A142" activeCellId="0" sqref="A142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B52" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+      <selection pane="topRight" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="2" style="0" width="8.28"/>
@@ -5653,7 +5647,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="16.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23"/>
       <c r="B1" s="23" t="n">
         <v>2003</v>
@@ -5710,7 +5704,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>46</v>
       </c>
@@ -5736,7 +5730,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>47</v>
       </c>
@@ -5792,7 +5786,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>48</v>
       </c>
@@ -5821,7 +5815,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>49</v>
       </c>
@@ -5847,7 +5841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>50</v>
       </c>
@@ -5903,7 +5897,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>51</v>
       </c>
@@ -5923,7 +5917,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>52</v>
       </c>
@@ -5976,7 +5970,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>53</v>
       </c>
@@ -6023,7 +6017,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>54</v>
       </c>
@@ -6052,7 +6046,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>55</v>
       </c>
@@ -6090,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>56</v>
       </c>
@@ -6098,7 +6092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>57</v>
       </c>
@@ -6106,7 +6100,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>58</v>
       </c>
@@ -6153,7 +6147,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>59</v>
       </c>
@@ -6212,7 +6206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>60</v>
       </c>
@@ -6268,7 +6262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>61</v>
       </c>
@@ -6294,7 +6288,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>62</v>
       </c>
@@ -6350,7 +6344,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>63</v>
       </c>
@@ -6358,7 +6352,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>64</v>
       </c>
@@ -6411,7 +6405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>65</v>
       </c>
@@ -6461,7 +6455,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>66</v>
       </c>
@@ -6490,7 +6484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>67</v>
       </c>
@@ -6537,7 +6531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>68</v>
       </c>
@@ -6590,7 +6584,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>69</v>
       </c>
@@ -6646,7 +6640,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>70</v>
       </c>
@@ -6657,7 +6651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>71</v>
       </c>
@@ -6704,7 +6698,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>72</v>
       </c>
@@ -6712,7 +6706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>73</v>
       </c>
@@ -6768,7 +6762,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>74</v>
       </c>
@@ -6818,7 +6812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>75</v>
       </c>
@@ -6856,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>76</v>
       </c>
@@ -6864,7 +6858,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>77</v>
       </c>
@@ -6896,7 +6890,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>78</v>
       </c>
@@ -6925,7 +6919,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>79</v>
       </c>
@@ -6984,7 +6978,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>80</v>
       </c>
@@ -7037,7 +7031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>81</v>
       </c>
@@ -7090,7 +7084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>82</v>
       </c>
@@ -7149,7 +7143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>83</v>
       </c>
@@ -7178,7 +7172,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>84</v>
       </c>
@@ -7228,7 +7222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>85</v>
       </c>
@@ -7287,7 +7281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>86</v>
       </c>
@@ -7316,7 +7310,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>87</v>
       </c>
@@ -7345,7 +7339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>88</v>
       </c>
@@ -7356,7 +7350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>89</v>
       </c>
@@ -7415,7 +7409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>90</v>
       </c>
@@ -7468,7 +7462,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>91</v>
       </c>
@@ -7521,7 +7515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>92</v>
       </c>
@@ -7571,7 +7565,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>93</v>
       </c>
@@ -7618,7 +7612,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>94</v>
       </c>
@@ -7677,7 +7671,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>95</v>
       </c>
@@ -7685,7 +7679,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>96</v>
       </c>
@@ -7732,7 +7726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>97</v>
       </c>
@@ -7788,7 +7782,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>98</v>
       </c>
@@ -7847,7 +7841,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>99</v>
       </c>
@@ -7864,7 +7858,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>100</v>
       </c>
@@ -7890,7 +7884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>101</v>
       </c>
@@ -7943,7 +7937,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>102</v>
       </c>
@@ -7990,7 +7984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>103</v>
       </c>
@@ -8043,7 +8037,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>104</v>
       </c>
@@ -8093,7 +8087,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>105</v>
       </c>
@@ -8143,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>106</v>
       </c>
@@ -8193,7 +8187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>107</v>
       </c>
@@ -8252,7 +8246,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>108</v>
       </c>
@@ -8299,7 +8293,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>109</v>
       </c>
@@ -8346,7 +8340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>110</v>
       </c>
@@ -8402,7 +8396,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>111</v>
       </c>
@@ -8449,7 +8443,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>112</v>
       </c>
@@ -8496,7 +8490,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>113</v>
       </c>
@@ -8555,7 +8549,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>114</v>
       </c>
@@ -8611,7 +8605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>115</v>
       </c>
@@ -8670,7 +8664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>116</v>
       </c>
@@ -8714,7 +8708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>117</v>
       </c>
@@ -8761,7 +8755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>118</v>
       </c>
@@ -8817,7 +8811,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>119</v>
       </c>
@@ -8861,162 +8855,150 @@
         <v>0</v>
       </c>
       <c r="O75" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P75" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q75" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R75" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S75" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>120</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J76" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K76" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L76" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M76" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N76" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O76" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="P76" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q76" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="R76" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="S76" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>121</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="C77" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="I77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J77" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K77" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L77" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="M77" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N77" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="O77" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P77" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q77" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="R77" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="S77" s="0" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>122</v>
       </c>
       <c r="B78" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>123</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G79" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H79" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I79" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J79" s="0" t="n">
         <v>0</v>
@@ -9037,112 +9019,118 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>124</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G80" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H80" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I80" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J80" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="K80" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L80" s="0" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="M80" s="0" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="N80" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O80" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+      <c r="P80" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>125</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G81" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H81" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I81" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J81" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="K81" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="L81" s="0" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="M81" s="0" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="N81" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="O81" s="0" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="P81" s="0" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>126</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0</v>
@@ -9157,113 +9145,104 @@
         <v>0</v>
       </c>
       <c r="H82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N82" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O82" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P82" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q82" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>127</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G83" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H83" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="I83" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="J83" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="K83" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="L83" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="M83" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="N83" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="O83" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>128</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="E84" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="G84" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="H84" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="I84" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J84" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="K84" s="0" t="n">
         <v>70</v>
@@ -9278,62 +9257,77 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>129</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="G85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="H85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="I85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="J85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="K85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="L85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="M85" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="N85" s="0" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="O85" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="P85" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q85" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="R85" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="S85" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>130</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>10</v>
@@ -9345,63 +9339,57 @@
         <v>10</v>
       </c>
       <c r="H86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N86" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O86" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="P86" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q86" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="R86" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="S86" s="0" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>131</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G87" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H87" s="0" t="n">
         <v>0</v>
@@ -9425,16 +9413,19 @@
         <v>0</v>
       </c>
       <c r="O87" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P87" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q87" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="R87" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>132</v>
       </c>
@@ -9478,19 +9469,22 @@
         <v>0</v>
       </c>
       <c r="O88" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P88" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q88" s="0" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R88" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="S88" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>133</v>
       </c>
@@ -9513,16 +9507,16 @@
         <v>0</v>
       </c>
       <c r="H89" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I89" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J89" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K89" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L89" s="0" t="n">
         <v>0</v>
@@ -9540,13 +9534,10 @@
         <v>0</v>
       </c>
       <c r="Q89" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R89" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>134</v>
       </c>
@@ -9590,22 +9581,16 @@
         <v>0</v>
       </c>
       <c r="O90" s="0" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="P90" s="0" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="Q90" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R90" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S90" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>135</v>
       </c>
@@ -9628,37 +9613,31 @@
         <v>0</v>
       </c>
       <c r="H91" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I91" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J91" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K91" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L91" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M91" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N91" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O91" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P91" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q91" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>136</v>
       </c>
@@ -9681,7 +9660,7 @@
         <v>0</v>
       </c>
       <c r="H92" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I92" s="0" t="n">
         <v>0</v>
@@ -9702,16 +9681,22 @@
         <v>0</v>
       </c>
       <c r="O92" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R92" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="P92" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="Q92" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S92" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>137</v>
       </c>
@@ -9734,31 +9719,34 @@
         <v>0</v>
       </c>
       <c r="H93" s="0" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I93" s="0" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J93" s="0" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="K93" s="0" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="L93" s="0" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="M93" s="0" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="N93" s="0" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="O93" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="P93" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>138</v>
       </c>
@@ -9781,7 +9769,7 @@
         <v>0</v>
       </c>
       <c r="H94" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I94" s="0" t="n">
         <v>0</v>
@@ -9796,28 +9784,25 @@
         <v>0</v>
       </c>
       <c r="M94" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="N94" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O94" s="0" t="n">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="P94" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="Q94" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="R94" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="S94" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>139</v>
       </c>
@@ -9840,34 +9825,40 @@
         <v>0</v>
       </c>
       <c r="H95" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I95" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J95" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K95" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="L95" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="M95" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="N95" s="0" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="O95" s="0" t="n">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="P95" s="0" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="Q95" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="R95" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>140</v>
       </c>
@@ -9905,81 +9896,81 @@
         <v>0</v>
       </c>
       <c r="M96" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="N96" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="O96" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P96" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q96" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="R96" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>141</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G97" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H97" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I97" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J97" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K97" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L97" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M97" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N97" s="0" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O97" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="P97" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="Q97" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="R97" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="S97" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="R97" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>142</v>
       </c>
@@ -10020,125 +10011,119 @@
         <v>0</v>
       </c>
       <c r="N98" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O98" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="P98" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="Q98" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="R98" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="S98" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G99" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H99" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I99" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="J99" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K99" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L99" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M99" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N99" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="O99" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P99" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="R99" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="S99" s="0" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>144</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="K100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="L100" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M100" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N100" s="0" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="O100" s="0" t="n">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="P100" s="0" t="n">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="Q100" s="0" t="n">
         <v>95</v>
@@ -10147,10 +10132,10 @@
         <v>95</v>
       </c>
       <c r="S100" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>145</v>
       </c>
@@ -10191,128 +10176,128 @@
         <v>0</v>
       </c>
       <c r="N101" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O101" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+      <c r="P101" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q101" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="R101" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>146</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H102" s="0" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="I102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="L102" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="M102" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="N102" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="O102" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="P102" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="Q102" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="R102" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="S102" s="0" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>147</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J103" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K103" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L103" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M103" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N103" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O103" s="0" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="P103" s="0" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="Q103" s="0" t="n">
         <v>95</v>
       </c>
       <c r="R103" s="0" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="S103" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>148</v>
       </c>
@@ -10323,7 +10308,7 @@
         <v>0</v>
       </c>
       <c r="D104" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>0</v>
@@ -10335,7 +10320,7 @@
         <v>0</v>
       </c>
       <c r="H104" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I104" s="0" t="n">
         <v>0</v>
@@ -10356,18 +10341,24 @@
         <v>0</v>
       </c>
       <c r="O104" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P104" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q104" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>149</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>15</v>
@@ -10379,46 +10370,34 @@
         <v>15</v>
       </c>
       <c r="G105" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H105" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I105" s="0" t="n">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="J105" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K105" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L105" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M105" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N105" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O105" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="P105" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="Q105" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="R105" s="0" t="n">
-        <v>85</v>
-      </c>
-      <c r="S105" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>150</v>
       </c>
@@ -10441,84 +10420,84 @@
         <v>0</v>
       </c>
       <c r="H106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="K106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="M106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="N106" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O106" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P106" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q106" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>151</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D107" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G107" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="H107" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I107" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="J107" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K107" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="E107" s="0" t="n">
+      <c r="L107" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F107" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G107" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H107" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I107" s="0" t="n">
+      <c r="M107" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N107" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P107" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q107" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="J107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O107" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>152</v>
       </c>
@@ -10541,66 +10520,45 @@
         <v>0</v>
       </c>
       <c r="H108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="J108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="K108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="M108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="N108" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="O108" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>153</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G109" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H109" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="I109" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J109" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K109" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L109" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M109" s="0" t="n">
         <v>0</v>
@@ -10609,16 +10567,16 @@
         <v>0</v>
       </c>
       <c r="O109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="P109" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q109" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>154</v>
       </c>
@@ -10641,10 +10599,40 @@
         <v>0</v>
       </c>
       <c r="H110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R110" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>155</v>
       </c>
@@ -10684,28 +10672,16 @@
       <c r="M111" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N111" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O111" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P111" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q111" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>156</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D112" s="0" t="n">
         <v>0</v>
@@ -10714,10 +10690,10 @@
         <v>0</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G112" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H112" s="0" t="n">
         <v>0</v>
@@ -10735,25 +10711,25 @@
         <v>0</v>
       </c>
       <c r="M112" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N112" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O112" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P112" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q112" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="R112" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>157</v>
       </c>
@@ -10779,30 +10755,48 @@
         <v>0</v>
       </c>
       <c r="I113" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J113" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K113" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L113" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M113" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N113" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O113" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P113" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q113" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="R113" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="S113" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C114" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D114" s="0" t="n">
         <v>0</v>
@@ -10811,10 +10805,10 @@
         <v>0</v>
       </c>
       <c r="F114" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G114" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H114" s="0" t="n">
         <v>0</v>
@@ -10832,25 +10826,16 @@
         <v>0</v>
       </c>
       <c r="M114" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N114" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O114" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="P114" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q114" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R114" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>159</v>
       </c>
@@ -10876,40 +10861,25 @@
         <v>0</v>
       </c>
       <c r="I115" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J115" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K115" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L115" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M115" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N115" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O115" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="P115" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q115" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="R115" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="S115" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>160</v>
       </c>
@@ -10950,27 +10920,39 @@
         <v>0</v>
       </c>
       <c r="N116" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O116" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="P116" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q116" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="R116" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="S116" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>161</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C117" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E117" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F117" s="0" t="n">
         <v>0</v>
@@ -10985,22 +10967,37 @@
         <v>0</v>
       </c>
       <c r="J117" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K117" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L117" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M117" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N117" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="O117" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="P117" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q117" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="R117" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S117" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>162</v>
       </c>
@@ -11044,36 +11041,33 @@
         <v>0</v>
       </c>
       <c r="O118" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="P118" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q118" s="0" t="n">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="R118" s="0" t="n">
-        <v>85</v>
-      </c>
-      <c r="S118" s="0" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>163</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C119" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E119" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F119" s="0" t="n">
         <v>0</v>
@@ -11087,38 +11081,8 @@
       <c r="I119" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J119" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K119" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L119" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M119" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N119" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O119" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="P119" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="Q119" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="R119" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="S119" s="0" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>164</v>
       </c>
@@ -11144,45 +11108,48 @@
         <v>0</v>
       </c>
       <c r="I120" s="0" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="J120" s="0" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="K120" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L120" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M120" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N120" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O120" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="P120" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q120" s="0" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="R120" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="S120" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>165</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C121" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D121" s="0" t="n">
         <v>0</v>
@@ -11194,83 +11161,101 @@
         <v>0</v>
       </c>
       <c r="G121" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H121" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I121" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="J121" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K121" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L121" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="M121" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N121" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O121" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="P121" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q121" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="R121" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="S121" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E122" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G122" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H122" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I122" s="0" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="J122" s="0" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="K122" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L122" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M122" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="N122" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="O122" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="P122" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q122" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="R122" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="S122" s="0" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>167</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D123" s="0" t="n">
         <v>0</v>
@@ -11282,93 +11267,96 @@
         <v>0</v>
       </c>
       <c r="G123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H123" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I123" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J123" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N123" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O123" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="P123" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="Q123" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="R123" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="S123" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>168</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C124" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D124" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I124" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="N124" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="F124" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G124" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H124" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I124" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J124" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="K124" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L124" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="M124" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N124" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="O124" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="P124" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q124" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>169</v>
       </c>
@@ -11412,19 +11400,16 @@
         <v>0</v>
       </c>
       <c r="O125" s="0" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="P125" s="0" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q125" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R125" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>170</v>
       </c>
@@ -11447,10 +11432,10 @@
         <v>0</v>
       </c>
       <c r="H126" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I126" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J126" s="0" t="n">
         <v>0</v>
@@ -11462,22 +11447,22 @@
         <v>0</v>
       </c>
       <c r="M126" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="N126" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="O126" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P126" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q126" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>171</v>
       </c>
@@ -11500,10 +11485,10 @@
         <v>0</v>
       </c>
       <c r="H127" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I127" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J127" s="0" t="n">
         <v>0</v>
@@ -11515,30 +11500,36 @@
         <v>0</v>
       </c>
       <c r="M127" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N127" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O127" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P127" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q127" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="R127" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="S127" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>172</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D128" s="0" t="n">
         <v>0</v>
@@ -11553,7 +11544,7 @@
         <v>0</v>
       </c>
       <c r="H128" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I128" s="0" t="n">
         <v>0</v>
@@ -11574,16 +11565,10 @@
         <v>0</v>
       </c>
       <c r="O128" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P128" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q128" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>173</v>
       </c>
@@ -11606,10 +11591,10 @@
         <v>0</v>
       </c>
       <c r="H129" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I129" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J129" s="0" t="n">
         <v>0</v>
@@ -11621,36 +11606,36 @@
         <v>0</v>
       </c>
       <c r="M129" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N129" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O129" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="P129" s="0" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="Q129" s="0" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="R129" s="0" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S129" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>174</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C130" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>0</v>
@@ -11665,101 +11650,80 @@
         <v>0</v>
       </c>
       <c r="H130" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O130" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>175</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E131" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G131" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H131" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I131" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J131" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K131" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L131" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M131" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N131" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O131" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="P131" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q131" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="R131" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="S131" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="R131" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="S131" s="0" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>176</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>0</v>
@@ -11773,46 +11737,64 @@
       <c r="H132" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>177</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E133" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G133" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H133" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="I133" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J133" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K133" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L133" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M133" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="N133" s="0" t="n">
         <v>0</v>
@@ -11824,27 +11806,21 @@
         <v>0</v>
       </c>
       <c r="Q133" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="R133" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="S133" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>178</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C134" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>0</v>
@@ -11874,10 +11850,25 @@
         <v>0</v>
       </c>
       <c r="N134" s="0" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="O134" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="R134" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="S134" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>179</v>
       </c>
@@ -11921,16 +11912,22 @@
         <v>0</v>
       </c>
       <c r="O135" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P135" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q135" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="R135" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="S135" s="0" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>180</v>
       </c>
@@ -11974,22 +11971,22 @@
         <v>0</v>
       </c>
       <c r="O136" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P136" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q136" s="0" t="n">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="R136" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="S136" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>181</v>
       </c>
@@ -12030,13 +12027,13 @@
         <v>0</v>
       </c>
       <c r="N137" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O137" s="0" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="P137" s="0" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="Q137" s="0" t="n">
         <v>90</v>
@@ -12045,10 +12042,10 @@
         <v>90</v>
       </c>
       <c r="S137" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>182</v>
       </c>
@@ -12086,28 +12083,28 @@
         <v>0</v>
       </c>
       <c r="M138" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N138" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O138" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P138" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Q138" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="R138" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="S138" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>183</v>
       </c>
@@ -12148,162 +12145,31 @@
         <v>0</v>
       </c>
       <c r="N139" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O139" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="P139" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q139" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="R139" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="S139" s="0" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M140" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O140" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="P140" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q140" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R140" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="S140" s="0" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S141" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="7"/>
-    </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="7"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>